<commit_message>
Remplace word doc par pdf
Ajustement des COLA en décimales et remplace document-source en word par pdf.
</commit_message>
<xml_diff>
--- a/params/cpp_history.xlsx
+++ b/params/cpp_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeielonelmezil/cpp/params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20472C1-3611-0C42-9597-38E0158BAA7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0024BC1F-964A-644E-ABD4-A96B0C13E858}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17900" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17900" windowHeight="16560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cppyear" sheetId="1" r:id="rId1"/>
@@ -1232,11 +1232,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T58" sqref="T58"/>
+      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8889,10 +8889,10 @@
   <dimension ref="A1:AC68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="AC2" sqref="AC2:AC54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9077,7 +9077,7 @@
       <c r="AB2" s="39">
         <v>0</v>
       </c>
-      <c r="AC2" s="39">
+      <c r="AC2" s="42">
         <v>0</v>
       </c>
     </row>
@@ -9167,7 +9167,7 @@
       <c r="AB3" s="39">
         <v>0</v>
       </c>
-      <c r="AC3" s="39">
+      <c r="AC3" s="42">
         <v>0</v>
       </c>
     </row>
@@ -9257,8 +9257,8 @@
       <c r="AB4" s="39">
         <v>0</v>
       </c>
-      <c r="AC4" s="39">
-        <v>2</v>
+      <c r="AC4" s="42">
+        <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9347,8 +9347,8 @@
       <c r="AB5" s="39">
         <v>0</v>
       </c>
-      <c r="AC5" s="39">
-        <v>2</v>
+      <c r="AC5" s="42">
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9437,8 +9437,8 @@
       <c r="AB6" s="39">
         <v>26.53</v>
       </c>
-      <c r="AC6" s="39">
-        <v>2</v>
+      <c r="AC6" s="42">
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9527,8 +9527,8 @@
       <c r="AB7" s="39">
         <v>27.06</v>
       </c>
-      <c r="AC7" s="39">
-        <v>2</v>
+      <c r="AC7" s="42">
+        <v>0.02</v>
       </c>
     </row>
     <row r="8" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9617,8 +9617,8 @@
       <c r="AB8" s="39">
         <v>80</v>
       </c>
-      <c r="AC8" s="39">
-        <v>2</v>
+      <c r="AC8" s="42">
+        <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9707,8 +9707,8 @@
       <c r="AB9" s="39">
         <v>86.56</v>
       </c>
-      <c r="AC9" s="39">
-        <v>3</v>
+      <c r="AC9" s="42">
+        <v>0.03</v>
       </c>
     </row>
     <row r="10" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9797,8 +9797,8 @@
       <c r="AB10" s="39">
         <v>95.59</v>
       </c>
-      <c r="AC10" s="39">
-        <v>8.1999999999999993</v>
+      <c r="AC10" s="42">
+        <v>8.199999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9887,8 +9887,8 @@
       <c r="AB11" s="39">
         <v>106.26</v>
       </c>
-      <c r="AC11" s="39">
-        <v>10.4</v>
+      <c r="AC11" s="42">
+        <v>0.10400000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -9977,8 +9977,8 @@
       <c r="AB12" s="39">
         <v>114.96</v>
       </c>
-      <c r="AC12" s="39">
-        <v>11.2</v>
+      <c r="AC12" s="42">
+        <v>0.11199999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10067,8 +10067,8 @@
       <c r="AB13" s="39">
         <v>123.56</v>
       </c>
-      <c r="AC13" s="39">
-        <v>8.1999999999999993</v>
+      <c r="AC13" s="42">
+        <v>8.199999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10157,8 +10157,8 @@
       <c r="AB14" s="39">
         <v>134.63999999999999</v>
       </c>
-      <c r="AC14" s="39">
-        <v>7.5</v>
+      <c r="AC14" s="42">
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="15" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10247,8 +10247,8 @@
       <c r="AB15" s="39">
         <v>146.78</v>
       </c>
-      <c r="AC15" s="39">
-        <v>9</v>
+      <c r="AC15" s="42">
+        <v>0.09</v>
       </c>
     </row>
     <row r="16" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10337,8 +10337,8 @@
       <c r="AB16" s="39">
         <v>161.31</v>
       </c>
-      <c r="AC16" s="39">
-        <v>9</v>
+      <c r="AC16" s="42">
+        <v>0.09</v>
       </c>
     </row>
     <row r="17" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10427,8 +10427,8 @@
       <c r="AB17" s="39">
         <v>181.18</v>
       </c>
-      <c r="AC17" s="39">
-        <v>9.9</v>
+      <c r="AC17" s="42">
+        <v>9.9000000000000005E-2</v>
       </c>
     </row>
     <row r="18" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10517,8 +10517,8 @@
       <c r="AB18" s="39">
         <v>201.44</v>
       </c>
-      <c r="AC18" s="39">
-        <v>12.3</v>
+      <c r="AC18" s="42">
+        <v>0.12300000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10607,8 +10607,8 @@
       <c r="AB19" s="39">
         <v>214.94</v>
       </c>
-      <c r="AC19" s="39">
-        <v>11.2</v>
+      <c r="AC19" s="42">
+        <v>0.11199999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10697,8 +10697,8 @@
       <c r="AB20" s="39">
         <v>224.4</v>
       </c>
-      <c r="AC20" s="39">
-        <v>6.7</v>
+      <c r="AC20" s="42">
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="21" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10787,8 +10787,8 @@
       <c r="AB21" s="39">
         <v>233.4</v>
       </c>
-      <c r="AC21" s="39">
-        <v>4.4000000000000004</v>
+      <c r="AC21" s="42">
+        <v>4.4000000000000004E-2</v>
       </c>
     </row>
     <row r="22" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10877,8 +10877,8 @@
       <c r="AB22" s="39">
         <v>242.95</v>
       </c>
-      <c r="AC22" s="39">
-        <v>4</v>
+      <c r="AC22" s="42">
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -10967,8 +10967,8 @@
       <c r="AB23" s="39">
         <v>253.64</v>
       </c>
-      <c r="AC23" s="39">
-        <v>4.0999999999999996</v>
+      <c r="AC23" s="42">
+        <v>4.0999999999999995E-2</v>
       </c>
     </row>
     <row r="24" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11057,8 +11057,8 @@
       <c r="AB24" s="39">
         <v>264.04000000000002</v>
       </c>
-      <c r="AC24" s="39">
-        <v>4.4000000000000004</v>
+      <c r="AC24" s="42">
+        <v>4.4000000000000004E-2</v>
       </c>
     </row>
     <row r="25" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11147,8 +11147,8 @@
       <c r="AB25" s="39">
         <v>276.70999999999998</v>
       </c>
-      <c r="AC25" s="39">
-        <v>4.0999999999999996</v>
+      <c r="AC25" s="42">
+        <v>4.0999999999999995E-2</v>
       </c>
     </row>
     <row r="26" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11237,8 +11237,8 @@
       <c r="AB26" s="39">
         <v>289.99</v>
       </c>
-      <c r="AC26" s="39">
-        <v>4.8</v>
+      <c r="AC26" s="42">
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11327,8 +11327,8 @@
       <c r="AB27" s="39">
         <v>306.81</v>
       </c>
-      <c r="AC27" s="39">
-        <v>4.8</v>
+      <c r="AC27" s="42">
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11417,8 +11417,8 @@
       <c r="AB28" s="39">
         <v>312.33</v>
       </c>
-      <c r="AC28" s="39">
-        <v>5.8</v>
+      <c r="AC28" s="42">
+        <v>5.7999999999999996E-2</v>
       </c>
     </row>
     <row r="29" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11507,8 +11507,8 @@
       <c r="AB29" s="39">
         <v>318.26</v>
       </c>
-      <c r="AC29" s="39">
-        <v>1.8</v>
+      <c r="AC29" s="42">
+        <v>1.8000000000000002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11597,8 +11597,8 @@
       <c r="AB30" s="39">
         <v>318.26</v>
       </c>
-      <c r="AC30" s="39">
-        <v>1.9</v>
+      <c r="AC30" s="42">
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="31" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11687,7 +11687,7 @@
       <c r="AB31" s="39">
         <v>325.58</v>
       </c>
-      <c r="AC31" s="39">
+      <c r="AC31" s="42">
         <v>0</v>
       </c>
     </row>
@@ -11777,8 +11777,8 @@
       <c r="AB32" s="39">
         <v>330.46</v>
       </c>
-      <c r="AC32" s="39">
-        <v>2.2999999999999998</v>
+      <c r="AC32" s="42">
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="33" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11867,8 +11867,8 @@
       <c r="AB33" s="39">
         <v>336.74</v>
       </c>
-      <c r="AC33" s="39">
-        <v>1.5</v>
+      <c r="AC33" s="42">
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -11957,8 +11957,8 @@
       <c r="AB34" s="39">
         <v>339.77</v>
       </c>
-      <c r="AC34" s="39">
-        <v>1.9</v>
+      <c r="AC34" s="42">
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="35" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12047,8 +12047,8 @@
       <c r="AB35" s="39">
         <v>345.21</v>
       </c>
-      <c r="AC35" s="39">
-        <v>0.9</v>
+      <c r="AC35" s="42">
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="36" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12137,8 +12137,8 @@
       <c r="AB36" s="39">
         <v>353.84</v>
       </c>
-      <c r="AC36" s="39">
-        <v>1.6</v>
+      <c r="AC36" s="42">
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="37" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12227,8 +12227,8 @@
       <c r="AB37" s="39">
         <v>364.46</v>
       </c>
-      <c r="AC37" s="39">
-        <v>2.5</v>
+      <c r="AC37" s="42">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12317,8 +12317,8 @@
       <c r="AB38" s="39">
         <v>370.29</v>
       </c>
-      <c r="AC38" s="39">
-        <v>3</v>
+      <c r="AC38" s="42">
+        <v>0.03</v>
       </c>
     </row>
     <row r="39" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12407,8 +12407,8 @@
       <c r="AB39" s="39">
         <v>382.14</v>
       </c>
-      <c r="AC39" s="39">
-        <v>1.6</v>
+      <c r="AC39" s="42">
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="40" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12497,8 +12497,8 @@
       <c r="AB40" s="39">
         <v>388.64</v>
       </c>
-      <c r="AC40" s="39">
-        <v>3.2</v>
+      <c r="AC40" s="42">
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12587,8 +12587,8 @@
       <c r="AB41" s="39">
         <v>397.58</v>
       </c>
-      <c r="AC41" s="39">
-        <v>1.7</v>
+      <c r="AC41" s="42">
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12677,8 +12677,8 @@
       <c r="AB42" s="39">
         <v>405.93</v>
       </c>
-      <c r="AC42" s="39">
-        <v>2.2999999999999998</v>
+      <c r="AC42" s="42">
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="43" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12767,8 +12767,8 @@
       <c r="AB43" s="39">
         <v>414.05</v>
       </c>
-      <c r="AC43" s="39">
-        <v>2.1</v>
+      <c r="AC43" s="42">
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="44" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12857,8 +12857,8 @@
       <c r="AB44" s="39">
         <v>424.4</v>
       </c>
-      <c r="AC44" s="39">
-        <v>2</v>
+      <c r="AC44" s="42">
+        <v>0.02</v>
       </c>
     </row>
     <row r="45" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -12947,8 +12947,8 @@
       <c r="AB45" s="39">
         <v>426.1</v>
       </c>
-      <c r="AC45" s="39">
-        <v>2.5</v>
+      <c r="AC45" s="42">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13037,8 +13037,8 @@
       <c r="AB46" s="39">
         <v>433.34</v>
       </c>
-      <c r="AC46" s="39">
-        <v>0.4</v>
+      <c r="AC46" s="42">
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="47" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13127,8 +13127,8 @@
       <c r="AB47" s="39">
         <v>445.47</v>
       </c>
-      <c r="AC47" s="39">
-        <v>1.7</v>
+      <c r="AC47" s="42">
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13217,8 +13217,8 @@
       <c r="AB48" s="39">
         <v>453.49</v>
       </c>
-      <c r="AC48" s="39">
-        <v>2.8</v>
+      <c r="AC48" s="42">
+        <v>2.7999999999999997E-2</v>
       </c>
     </row>
     <row r="49" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13307,8 +13307,8 @@
       <c r="AB49" s="39">
         <v>457.57</v>
       </c>
-      <c r="AC49" s="39">
-        <v>1.8</v>
+      <c r="AC49" s="42">
+        <v>1.8000000000000002E-2</v>
       </c>
     </row>
     <row r="50" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13397,8 +13397,8 @@
       <c r="AB50" s="39">
         <v>465.81</v>
       </c>
-      <c r="AC50" s="39">
-        <v>0.9</v>
+      <c r="AC50" s="42">
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="51" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13487,8 +13487,8 @@
       <c r="AB51" s="39">
         <v>471.4</v>
       </c>
-      <c r="AC51" s="39">
-        <v>1.8</v>
+      <c r="AC51" s="42">
+        <v>1.8000000000000002E-2</v>
       </c>
     </row>
     <row r="52" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13577,8 +13577,8 @@
       <c r="AB52" s="39">
         <v>471.4</v>
       </c>
-      <c r="AC52" s="39">
-        <v>1.2</v>
+      <c r="AC52" s="42">
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="53" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13667,8 +13667,8 @@
       <c r="AB53" s="39">
         <v>478</v>
       </c>
-      <c r="AC53" s="39">
-        <v>1.4</v>
+      <c r="AC53" s="42">
+        <v>1.3999999999999999E-2</v>
       </c>
     </row>
     <row r="54" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13757,8 +13757,8 @@
       <c r="AB54" s="39">
         <v>485.17</v>
       </c>
-      <c r="AC54" s="39">
-        <v>1.5</v>
+      <c r="AC54" s="42">
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="55" spans="1:29" s="42" customFormat="1" x14ac:dyDescent="0.2">
@@ -13839,8 +13839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F9A59A-0B8E-6B4A-B1EF-17468881AF9E}">
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="P9" sqref="P9:P11"/>
@@ -14317,7 +14317,7 @@
       </c>
       <c r="AC4" s="2">
         <f>cppyear!AC4-qpp!AC4</f>
-        <v>-1.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -14435,7 +14435,7 @@
       </c>
       <c r="AC5" s="2">
         <f>cppyear!AC5-qpp!AC5</f>
-        <v>-1.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -14553,7 +14553,7 @@
       </c>
       <c r="AC6" s="2">
         <f>cppyear!AC6-qpp!AC6</f>
-        <v>-1.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -14671,7 +14671,7 @@
       </c>
       <c r="AC7" s="2">
         <f>cppyear!AC7-qpp!AC7</f>
-        <v>-1.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -14789,7 +14789,7 @@
       </c>
       <c r="AC8" s="2">
         <f>cppyear!AC8-qpp!AC8</f>
-        <v>-1.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -14907,7 +14907,7 @@
       </c>
       <c r="AC9" s="2">
         <f>cppyear!AC9-qpp!AC9</f>
-        <v>-2.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -15025,7 +15025,7 @@
       </c>
       <c r="AC10" s="2">
         <f>cppyear!AC10-qpp!AC10</f>
-        <v>-8.1179999999999986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -15143,7 +15143,7 @@
       </c>
       <c r="AC11" s="2">
         <f>cppyear!AC11-qpp!AC11</f>
-        <v>-10.296000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -15261,7 +15261,7 @@
       </c>
       <c r="AC12" s="2">
         <f>cppyear!AC12-qpp!AC12</f>
-        <v>-11.087999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -15379,7 +15379,7 @@
       </c>
       <c r="AC13" s="2">
         <f>cppyear!AC13-qpp!AC13</f>
-        <v>-8.1179999999999986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -15497,7 +15497,7 @@
       </c>
       <c r="AC14" s="2">
         <f>cppyear!AC14-qpp!AC14</f>
-        <v>-7.4249999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -15615,7 +15615,7 @@
       </c>
       <c r="AC15" s="2">
         <f>cppyear!AC15-qpp!AC15</f>
-        <v>-8.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -15733,7 +15733,7 @@
       </c>
       <c r="AC16" s="2">
         <f>cppyear!AC16-qpp!AC16</f>
-        <v>-8.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -15851,7 +15851,7 @@
       </c>
       <c r="AC17" s="2">
         <f>cppyear!AC17-qpp!AC17</f>
-        <v>-9.8010000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -15969,7 +15969,7 @@
       </c>
       <c r="AC18" s="2">
         <f>cppyear!AC18-qpp!AC18</f>
-        <v>-12.177000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
@@ -16087,7 +16087,7 @@
       </c>
       <c r="AC19" s="2">
         <f>cppyear!AC19-qpp!AC19</f>
-        <v>-11.087999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
@@ -16205,7 +16205,7 @@
       </c>
       <c r="AC20" s="2">
         <f>cppyear!AC20-qpp!AC20</f>
-        <v>-6.633</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
@@ -16323,7 +16323,7 @@
       </c>
       <c r="AC21" s="2">
         <f>cppyear!AC21-qpp!AC21</f>
-        <v>-4.3560000000000008</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
@@ -16441,7 +16441,7 @@
       </c>
       <c r="AC22" s="2">
         <f>cppyear!AC22-qpp!AC22</f>
-        <v>-3.96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
@@ -16559,7 +16559,7 @@
       </c>
       <c r="AC23" s="2">
         <f>cppyear!AC23-qpp!AC23</f>
-        <v>-4.0589999999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
@@ -16677,7 +16677,7 @@
       </c>
       <c r="AC24" s="2">
         <f>cppyear!AC24-qpp!AC24</f>
-        <v>-4.3560000000000008</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
@@ -16795,7 +16795,7 @@
       </c>
       <c r="AC25" s="2">
         <f>cppyear!AC25-qpp!AC25</f>
-        <v>-4.0589999999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
@@ -16913,7 +16913,7 @@
       </c>
       <c r="AC26" s="2">
         <f>cppyear!AC26-qpp!AC26</f>
-        <v>-4.7519999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
@@ -17031,7 +17031,7 @@
       </c>
       <c r="AC27" s="2">
         <f>cppyear!AC27-qpp!AC27</f>
-        <v>-4.7519999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
@@ -17149,7 +17149,7 @@
       </c>
       <c r="AC28" s="2">
         <f>cppyear!AC28-qpp!AC28</f>
-        <v>-5.742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
@@ -17267,7 +17267,7 @@
       </c>
       <c r="AC29" s="2">
         <f>cppyear!AC29-qpp!AC29</f>
-        <v>-1.782</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
@@ -17385,7 +17385,7 @@
       </c>
       <c r="AC30" s="2">
         <f>cppyear!AC30-qpp!AC30</f>
-        <v>-1.881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
@@ -17621,7 +17621,7 @@
       </c>
       <c r="AC32" s="2">
         <f>cppyear!AC32-qpp!AC32</f>
-        <v>-2.282</v>
+        <v>-5.000000000000001E-3</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.2">
@@ -17739,7 +17739,7 @@
       </c>
       <c r="AC33" s="2">
         <f>cppyear!AC33-qpp!AC33</f>
-        <v>-1.4850000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.2">
@@ -17857,7 +17857,7 @@
       </c>
       <c r="AC34" s="2">
         <f>cppyear!AC34-qpp!AC34</f>
-        <v>-1.881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.2">
@@ -17975,7 +17975,7 @@
       </c>
       <c r="AC35" s="2">
         <f>cppyear!AC35-qpp!AC35</f>
-        <v>-0.89100000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
@@ -18093,7 +18093,7 @@
       </c>
       <c r="AC36" s="2">
         <f>cppyear!AC36-qpp!AC36</f>
-        <v>-1.5840000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
@@ -18211,7 +18211,7 @@
       </c>
       <c r="AC37" s="2">
         <f>cppyear!AC37-qpp!AC37</f>
-        <v>-2.4750000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.2">
@@ -18329,7 +18329,7 @@
       </c>
       <c r="AC38" s="2">
         <f>cppyear!AC38-qpp!AC38</f>
-        <v>-2.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
@@ -18447,7 +18447,7 @@
       </c>
       <c r="AC39" s="2">
         <f>cppyear!AC39-qpp!AC39</f>
-        <v>-1.5840000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
@@ -18565,7 +18565,7 @@
       </c>
       <c r="AC40" s="2">
         <f>cppyear!AC40-qpp!AC40</f>
-        <v>-3.1680000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
@@ -18683,7 +18683,7 @@
       </c>
       <c r="AC41" s="2">
         <f>cppyear!AC41-qpp!AC41</f>
-        <v>-1.6830000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.2">
@@ -18801,7 +18801,7 @@
       </c>
       <c r="AC42" s="2">
         <f>cppyear!AC42-qpp!AC42</f>
-        <v>-2.2769999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.2">
@@ -18919,7 +18919,7 @@
       </c>
       <c r="AC43" s="2">
         <f>cppyear!AC43-qpp!AC43</f>
-        <v>-2.0790000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.2">
@@ -19037,7 +19037,7 @@
       </c>
       <c r="AC44" s="2">
         <f>cppyear!AC44-qpp!AC44</f>
-        <v>-1.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
@@ -19155,7 +19155,7 @@
       </c>
       <c r="AC45" s="2">
         <f>cppyear!AC45-qpp!AC45</f>
-        <v>-2.4750000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
@@ -19273,7 +19273,7 @@
       </c>
       <c r="AC46" s="2">
         <f>cppyear!AC46-qpp!AC46</f>
-        <v>-0.39600000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.2">
@@ -19391,7 +19391,7 @@
       </c>
       <c r="AC47" s="2">
         <f>cppyear!AC47-qpp!AC47</f>
-        <v>-1.6830000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.2">
@@ -19509,7 +19509,7 @@
       </c>
       <c r="AC48" s="2">
         <f>cppyear!AC48-qpp!AC48</f>
-        <v>-2.7719999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
@@ -19627,7 +19627,7 @@
       </c>
       <c r="AC49" s="2">
         <f>cppyear!AC49-qpp!AC49</f>
-        <v>-1.782</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
@@ -19745,7 +19745,7 @@
       </c>
       <c r="AC50" s="2">
         <f>cppyear!AC50-qpp!AC50</f>
-        <v>-0.89100000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
@@ -19863,7 +19863,7 @@
       </c>
       <c r="AC51" s="2">
         <f>cppyear!AC51-qpp!AC51</f>
-        <v>-1.782</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.2">
@@ -19981,7 +19981,7 @@
       </c>
       <c r="AC52" s="2">
         <f>cppyear!AC52-qpp!AC52</f>
-        <v>-1.1879999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.2">
@@ -20099,7 +20099,7 @@
       </c>
       <c r="AC53" s="2">
         <f>cppyear!AC53-qpp!AC53</f>
-        <v>-1.3859999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.2">
@@ -20217,7 +20217,7 @@
       </c>
       <c r="AC54" s="2">
         <f>cppyear!AC54-qpp!AC54</f>
-        <v>-1.4850000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Split PRB in PRB, PRB_s1 and PRB_s2
Plusadd param for PRB in params files
</commit_message>
<xml_diff>
--- a/params/cpp_history.xlsx
+++ b/params/cpp_history.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Judith/Documents/GitHub/cpp/params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/UQAM/git/cpp/params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBEFF2E-B40B-9F42-84FD-4D73E7CB73D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="46120" windowHeight="25300"/>
   </bookViews>
   <sheets>
     <sheet name="cppyear" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>year</t>
   </si>
@@ -90,9 +95,6 @@
     <t>lra</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>supp</t>
   </si>
   <si>
@@ -143,11 +145,17 @@
   <si>
     <t>reprate_s2</t>
   </si>
+  <si>
+    <t>supp_s1</t>
+  </si>
+  <si>
+    <t>supp_s2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -642,7 +650,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -656,50 +664,53 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1010,26 +1021,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S71" sqref="S71"/>
+      <selection pane="bottomRight" activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="11" width="10.83203125" style="1"/>
     <col min="12" max="13" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="29" width="10.83203125" style="1"/>
-    <col min="32" max="32" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="28" width="10.83203125" style="1"/>
+    <col min="31" max="31" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1064,16 +1076,16 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>11</v>
@@ -1106,15 +1118,15 @@
         <v>20</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="10" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="10" t="s">
@@ -1141,11 +1153,14 @@
       <c r="AK1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AL1" s="13" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1966</v>
       </c>
@@ -1222,19 +1237,19 @@
         <v>0</v>
       </c>
       <c r="Z2" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA2" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -1257,11 +1272,14 @@
       <c r="AK2">
         <v>0</v>
       </c>
-      <c r="AL2">
+      <c r="AL2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1967</v>
       </c>
@@ -1338,19 +1356,19 @@
         <v>0</v>
       </c>
       <c r="Z3" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA3" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
       </c>
       <c r="AD3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3">
         <v>0</v>
@@ -1373,11 +1391,14 @@
       <c r="AK3">
         <v>0</v>
       </c>
-      <c r="AL3">
+      <c r="AL3" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1968</v>
       </c>
@@ -1454,19 +1475,19 @@
         <v>0</v>
       </c>
       <c r="Z4" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA4" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB4" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="5">
         <v>0.02</v>
       </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
       <c r="AD4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4">
         <v>0</v>
@@ -1489,11 +1510,14 @@
       <c r="AK4">
         <v>0</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1969</v>
       </c>
@@ -1570,19 +1594,19 @@
         <v>0</v>
       </c>
       <c r="Z5" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA5" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB5" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="5">
         <v>0.02</v>
       </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
       <c r="AD5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
         <v>0</v>
@@ -1605,11 +1629,14 @@
       <c r="AK5">
         <v>0</v>
       </c>
-      <c r="AL5">
+      <c r="AL5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1970</v>
       </c>
@@ -1686,19 +1713,19 @@
         <v>0</v>
       </c>
       <c r="Z6" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA6" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB6" s="6">
         <v>26.53</v>
       </c>
-      <c r="AC6" s="5">
+      <c r="AB6" s="5">
         <v>0.02</v>
       </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1721,11 +1748,14 @@
       <c r="AK6">
         <v>0</v>
       </c>
-      <c r="AL6">
+      <c r="AL6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1971</v>
       </c>
@@ -1802,19 +1832,19 @@
         <v>0</v>
       </c>
       <c r="Z7" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA7" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB7" s="6">
         <v>27.06</v>
       </c>
-      <c r="AC7" s="5">
+      <c r="AB7" s="5">
         <v>0.02</v>
       </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
       <c r="AD7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7">
         <v>0</v>
@@ -1837,11 +1867,14 @@
       <c r="AK7">
         <v>0</v>
       </c>
-      <c r="AL7">
+      <c r="AL7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1972</v>
       </c>
@@ -1918,19 +1951,19 @@
         <v>0</v>
       </c>
       <c r="Z8" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA8" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB8" s="6">
         <v>80</v>
       </c>
-      <c r="AC8" s="5">
+      <c r="AB8" s="5">
         <v>0.02</v>
       </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
       <c r="AD8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8">
         <v>0</v>
@@ -1953,11 +1986,14 @@
       <c r="AK8">
         <v>0</v>
       </c>
-      <c r="AL8">
+      <c r="AL8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1973</v>
       </c>
@@ -2034,19 +2070,19 @@
         <v>0</v>
       </c>
       <c r="Z9" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA9" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB9" s="6">
         <v>86.56</v>
       </c>
-      <c r="AC9" s="8">
+      <c r="AB9" s="8">
         <v>0.03</v>
       </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
       <c r="AD9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9">
         <v>0</v>
@@ -2069,11 +2105,14 @@
       <c r="AK9">
         <v>0</v>
       </c>
-      <c r="AL9">
+      <c r="AL9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1974</v>
       </c>
@@ -2150,19 +2189,19 @@
         <v>0</v>
       </c>
       <c r="Z10" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA10" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB10" s="6">
         <v>95.59</v>
       </c>
-      <c r="AC10" s="8">
+      <c r="AB10" s="8">
         <v>8.2000000000000003E-2</v>
       </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
       <c r="AD10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10">
         <v>0</v>
@@ -2185,11 +2224,14 @@
       <c r="AK10">
         <v>0</v>
       </c>
-      <c r="AL10">
+      <c r="AL10" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1975</v>
       </c>
@@ -2266,19 +2308,19 @@
         <v>0</v>
       </c>
       <c r="Z11" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA11" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB11" s="6">
         <v>106.26</v>
       </c>
-      <c r="AC11" s="8">
+      <c r="AB11" s="8">
         <v>0.104</v>
       </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
       <c r="AD11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE11">
         <v>0</v>
@@ -2301,11 +2343,14 @@
       <c r="AK11">
         <v>0</v>
       </c>
-      <c r="AL11">
+      <c r="AL11" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1976</v>
       </c>
@@ -2382,19 +2427,19 @@
         <v>0</v>
       </c>
       <c r="Z12" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA12" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB12" s="6">
         <v>114.96</v>
       </c>
-      <c r="AC12" s="8">
+      <c r="AB12" s="8">
         <v>0.112</v>
       </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
       <c r="AD12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE12">
         <v>0</v>
@@ -2417,11 +2462,14 @@
       <c r="AK12">
         <v>0</v>
       </c>
-      <c r="AL12">
+      <c r="AL12" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1977</v>
       </c>
@@ -2498,19 +2546,19 @@
         <v>0</v>
       </c>
       <c r="Z13" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA13" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB13" s="6">
         <v>123.56</v>
       </c>
-      <c r="AC13" s="8">
+      <c r="AB13" s="8">
         <v>8.2000000000000003E-2</v>
       </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
       <c r="AD13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE13">
         <v>0</v>
@@ -2533,11 +2581,14 @@
       <c r="AK13">
         <v>0</v>
       </c>
-      <c r="AL13">
+      <c r="AL13" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1978</v>
       </c>
@@ -2614,19 +2665,19 @@
         <v>0</v>
       </c>
       <c r="Z14" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA14" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB14" s="6">
         <v>134.63999999999999</v>
       </c>
-      <c r="AC14" s="8">
+      <c r="AB14" s="8">
         <v>7.4999999999999997E-2</v>
       </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
       <c r="AD14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE14">
         <v>0</v>
@@ -2649,11 +2700,14 @@
       <c r="AK14">
         <v>0</v>
       </c>
-      <c r="AL14">
+      <c r="AL14" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1979</v>
       </c>
@@ -2730,19 +2784,19 @@
         <v>0</v>
       </c>
       <c r="Z15" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA15" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB15" s="6">
         <v>146.78</v>
       </c>
-      <c r="AC15" s="8">
+      <c r="AB15" s="8">
         <v>0.09</v>
       </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
       <c r="AD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15">
         <v>0</v>
@@ -2765,11 +2819,14 @@
       <c r="AK15">
         <v>0</v>
       </c>
-      <c r="AL15">
+      <c r="AL15" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1980</v>
       </c>
@@ -2846,19 +2903,19 @@
         <v>0</v>
       </c>
       <c r="Z16" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA16" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB16" s="6">
         <v>161.31</v>
       </c>
-      <c r="AC16" s="8">
+      <c r="AB16" s="8">
         <v>0.09</v>
       </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
       <c r="AD16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE16">
         <v>0</v>
@@ -2881,11 +2938,14 @@
       <c r="AK16">
         <v>0</v>
       </c>
-      <c r="AL16">
+      <c r="AL16" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1981</v>
       </c>
@@ -2962,19 +3022,19 @@
         <v>0</v>
       </c>
       <c r="Z17" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA17" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB17" s="6">
         <v>181.18</v>
       </c>
-      <c r="AC17" s="8">
+      <c r="AB17" s="8">
         <v>9.9000000000000005E-2</v>
       </c>
+      <c r="AC17">
+        <v>1</v>
+      </c>
       <c r="AD17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17">
         <v>0</v>
@@ -2997,11 +3057,14 @@
       <c r="AK17">
         <v>0</v>
       </c>
-      <c r="AL17">
+      <c r="AL17" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1982</v>
       </c>
@@ -3078,19 +3141,19 @@
         <v>0</v>
       </c>
       <c r="Z18" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA18" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB18" s="6">
         <v>201.44</v>
       </c>
-      <c r="AC18" s="8">
+      <c r="AB18" s="8">
         <v>0.123</v>
       </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
       <c r="AD18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE18">
         <v>0</v>
@@ -3113,11 +3176,14 @@
       <c r="AK18">
         <v>0</v>
       </c>
-      <c r="AL18">
+      <c r="AL18" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>1983</v>
       </c>
@@ -3194,19 +3260,19 @@
         <v>0</v>
       </c>
       <c r="Z19" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA19" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB19" s="6">
         <v>214.94</v>
       </c>
-      <c r="AC19" s="8">
+      <c r="AB19" s="8">
         <v>0.112</v>
       </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
       <c r="AD19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE19">
         <v>0</v>
@@ -3229,11 +3295,14 @@
       <c r="AK19">
         <v>0</v>
       </c>
-      <c r="AL19">
+      <c r="AL19" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>1984</v>
       </c>
@@ -3310,19 +3379,19 @@
         <v>0</v>
       </c>
       <c r="Z20" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA20" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB20" s="6">
         <v>224.4</v>
       </c>
-      <c r="AC20" s="8">
+      <c r="AB20" s="8">
         <v>6.7000000000000004E-2</v>
       </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
       <c r="AD20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE20">
         <v>0</v>
@@ -3345,11 +3414,14 @@
       <c r="AK20">
         <v>0</v>
       </c>
-      <c r="AL20">
+      <c r="AL20" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>1985</v>
       </c>
@@ -3426,19 +3498,19 @@
         <v>0</v>
       </c>
       <c r="Z21" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA21" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB21" s="6">
         <v>233.4</v>
       </c>
-      <c r="AC21" s="8">
+      <c r="AB21" s="8">
         <v>4.3999999999999997E-2</v>
       </c>
+      <c r="AC21">
+        <v>1</v>
+      </c>
       <c r="AD21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE21">
         <v>0</v>
@@ -3461,11 +3533,14 @@
       <c r="AK21">
         <v>0</v>
       </c>
-      <c r="AL21">
+      <c r="AL21" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>1986</v>
       </c>
@@ -3542,19 +3617,19 @@
         <v>0</v>
       </c>
       <c r="Z22" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA22" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB22" s="6">
         <v>242.95</v>
       </c>
-      <c r="AC22" s="8">
+      <c r="AB22" s="8">
         <v>0.04</v>
       </c>
+      <c r="AC22">
+        <v>1</v>
+      </c>
       <c r="AD22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE22">
         <v>0</v>
@@ -3577,11 +3652,14 @@
       <c r="AK22">
         <v>0</v>
       </c>
-      <c r="AL22">
+      <c r="AL22" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>1987</v>
       </c>
@@ -3654,23 +3732,23 @@
       <c r="X23" s="6">
         <v>70</v>
       </c>
-      <c r="Y23" s="7">
-        <v>0.24163552123552121</v>
+      <c r="Y23" s="6">
+        <v>0</v>
       </c>
       <c r="Z23" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA23" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB23" s="6">
         <v>253.64</v>
       </c>
-      <c r="AC23" s="8">
+      <c r="AB23" s="8">
         <v>4.1000000000000002E-2</v>
       </c>
+      <c r="AC23">
+        <v>1</v>
+      </c>
       <c r="AD23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE23">
         <v>0</v>
@@ -3693,11 +3771,14 @@
       <c r="AK23">
         <v>0</v>
       </c>
-      <c r="AL23">
+      <c r="AL23" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>1988</v>
       </c>
@@ -3770,23 +3851,23 @@
       <c r="X24" s="6">
         <v>70</v>
       </c>
-      <c r="Y24" s="7">
-        <v>0.24591396226415091</v>
+      <c r="Y24" s="6">
+        <v>0</v>
       </c>
       <c r="Z24" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA24" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB24" s="6">
         <v>264.04000000000002</v>
       </c>
-      <c r="AC24" s="8">
+      <c r="AB24" s="8">
         <v>4.3999999999999997E-2</v>
       </c>
+      <c r="AC24">
+        <v>1</v>
+      </c>
       <c r="AD24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE24">
         <v>0</v>
@@ -3809,11 +3890,14 @@
       <c r="AK24">
         <v>0</v>
       </c>
-      <c r="AL24">
+      <c r="AL24" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>1989</v>
       </c>
@@ -3886,23 +3970,23 @@
       <c r="X25" s="6">
         <v>70</v>
       </c>
-      <c r="Y25" s="7">
-        <v>0.24097472924187724</v>
+      <c r="Y25" s="6">
+        <v>0</v>
       </c>
       <c r="Z25" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA25" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB25" s="6">
         <v>276.70999999999998</v>
       </c>
-      <c r="AC25" s="8">
+      <c r="AB25" s="8">
         <v>4.1000000000000002E-2</v>
       </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
       <c r="AD25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE25">
         <v>0</v>
@@ -3925,11 +4009,14 @@
       <c r="AK25">
         <v>0</v>
       </c>
-      <c r="AL25">
+      <c r="AL25" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>1990</v>
       </c>
@@ -4002,23 +4089,23 @@
       <c r="X26" s="6">
         <v>70</v>
       </c>
-      <c r="Y26" s="7">
-        <v>0.23961799307958478</v>
+      <c r="Y26" s="6">
+        <v>0</v>
       </c>
       <c r="Z26" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA26" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB26" s="6">
         <v>289.99</v>
       </c>
-      <c r="AC26" s="8">
+      <c r="AB26" s="8">
         <v>4.8000000000000001E-2</v>
       </c>
+      <c r="AC26">
+        <v>1</v>
+      </c>
       <c r="AD26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE26">
         <v>0</v>
@@ -4041,11 +4128,14 @@
       <c r="AK26">
         <v>0</v>
       </c>
-      <c r="AL26">
+      <c r="AL26" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>1991</v>
       </c>
@@ -4118,23 +4208,23 @@
       <c r="X27" s="6">
         <v>70</v>
       </c>
-      <c r="Y27" s="7">
-        <v>0.2379777049180328</v>
+      <c r="Y27" s="6">
+        <v>0</v>
       </c>
       <c r="Z27" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA27" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB27" s="6">
         <v>306.81</v>
       </c>
-      <c r="AC27" s="8">
+      <c r="AB27" s="8">
         <v>4.8000000000000001E-2</v>
       </c>
+      <c r="AC27">
+        <v>1</v>
+      </c>
       <c r="AD27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE27">
         <v>0</v>
@@ -4157,11 +4247,14 @@
       <c r="AK27">
         <v>0</v>
       </c>
-      <c r="AL27">
+      <c r="AL27" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>1992</v>
       </c>
@@ -4234,23 +4327,23 @@
       <c r="X28" s="6">
         <v>70</v>
       </c>
-      <c r="Y28" s="7">
-        <v>0.23705962732919253</v>
+      <c r="Y28" s="6">
+        <v>0</v>
       </c>
       <c r="Z28" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA28" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB28" s="6">
         <v>312.33</v>
       </c>
-      <c r="AC28" s="8">
+      <c r="AB28" s="8">
         <v>5.8000000000000003E-2</v>
       </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
       <c r="AD28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE28">
         <v>0</v>
@@ -4273,11 +4366,14 @@
       <c r="AK28">
         <v>0</v>
       </c>
-      <c r="AL28">
+      <c r="AL28" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>1993</v>
       </c>
@@ -4350,23 +4446,23 @@
       <c r="X29" s="6">
         <v>70</v>
       </c>
-      <c r="Y29" s="7">
-        <v>0.2397700598802395</v>
+      <c r="Y29" s="6">
+        <v>0</v>
       </c>
       <c r="Z29" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA29" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB29" s="6">
         <v>318.26</v>
       </c>
-      <c r="AC29" s="8">
+      <c r="AB29" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
       <c r="AD29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE29">
         <v>0</v>
@@ -4389,11 +4485,14 @@
       <c r="AK29">
         <v>0</v>
       </c>
-      <c r="AL29">
+      <c r="AL29" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>1994</v>
       </c>
@@ -4466,23 +4565,23 @@
       <c r="X30" s="6">
         <v>70</v>
       </c>
-      <c r="Y30" s="7">
-        <v>0.242246511627907</v>
+      <c r="Y30" s="6">
+        <v>0</v>
       </c>
       <c r="Z30" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA30" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB30" s="6">
         <v>318.26</v>
       </c>
-      <c r="AC30" s="8">
+      <c r="AB30" s="8">
         <v>1.9E-2</v>
       </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
       <c r="AD30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE30">
         <v>0</v>
@@ -4505,11 +4604,14 @@
       <c r="AK30">
         <v>0</v>
       </c>
-      <c r="AL30">
+      <c r="AL30" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>1995</v>
       </c>
@@ -4582,23 +4684,23 @@
       <c r="X31" s="6">
         <v>70</v>
       </c>
-      <c r="Y31" s="7">
-        <v>0.24522292263610315</v>
+      <c r="Y31" s="6">
+        <v>0</v>
       </c>
       <c r="Z31" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA31" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB31" s="6">
         <v>325.58</v>
       </c>
-      <c r="AC31" s="8">
+      <c r="AB31" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
+      <c r="AC31">
+        <v>1</v>
+      </c>
       <c r="AD31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE31">
         <v>0</v>
@@ -4621,11 +4723,14 @@
       <c r="AK31">
         <v>0</v>
       </c>
-      <c r="AL31">
+      <c r="AL31" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>1996</v>
       </c>
@@ -4698,23 +4803,23 @@
       <c r="X32" s="6">
         <v>70</v>
       </c>
-      <c r="Y32" s="7">
-        <v>0.24646779661016952</v>
+      <c r="Y32" s="6">
+        <v>0</v>
       </c>
       <c r="Z32" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA32" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB32" s="6">
         <v>330.46</v>
       </c>
-      <c r="AC32" s="8">
+      <c r="AB32" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
+      <c r="AC32">
+        <v>1</v>
+      </c>
       <c r="AD32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE32">
         <v>0</v>
@@ -4737,11 +4842,14 @@
       <c r="AK32">
         <v>0</v>
       </c>
-      <c r="AL32">
+      <c r="AL32" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>1997</v>
       </c>
@@ -4814,23 +4922,23 @@
       <c r="X33" s="6">
         <v>70</v>
       </c>
-      <c r="Y33" s="7">
-        <v>0.24697541899441339</v>
+      <c r="Y33" s="6">
+        <v>0</v>
       </c>
       <c r="Z33" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA33" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB33" s="6">
         <v>336.74</v>
       </c>
-      <c r="AC33" s="8">
+      <c r="AB33" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="AC33">
+        <v>1</v>
+      </c>
       <c r="AD33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE33">
         <v>0</v>
@@ -4853,11 +4961,14 @@
       <c r="AK33">
         <v>0</v>
       </c>
-      <c r="AL33">
+      <c r="AL33" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>1998</v>
       </c>
@@ -4930,23 +5041,23 @@
       <c r="X34" s="6">
         <v>70</v>
       </c>
-      <c r="Y34" s="7">
-        <v>0.24220813008130079</v>
+      <c r="Y34" s="6">
+        <v>0</v>
       </c>
       <c r="Z34" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA34" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB34" s="6">
         <v>339.77</v>
       </c>
-      <c r="AC34" s="8">
+      <c r="AB34" s="8">
         <v>1.9E-2</v>
       </c>
+      <c r="AC34">
+        <v>1</v>
+      </c>
       <c r="AD34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE34">
         <v>0</v>
@@ -4969,11 +5080,14 @@
       <c r="AK34">
         <v>0</v>
       </c>
-      <c r="AL34">
+      <c r="AL34" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>1999</v>
       </c>
@@ -5046,23 +5160,23 @@
       <c r="X35" s="6">
         <v>70</v>
       </c>
-      <c r="Y35" s="7">
-        <v>0.24117754010695186</v>
+      <c r="Y35" s="6">
+        <v>0</v>
       </c>
       <c r="Z35" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA35" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB35" s="6">
         <v>345.21</v>
       </c>
-      <c r="AC35" s="8">
+      <c r="AB35" s="8">
         <v>8.9999999999999993E-3</v>
       </c>
+      <c r="AC35">
+        <v>1</v>
+      </c>
       <c r="AD35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE35">
         <v>0</v>
@@ -5085,11 +5199,14 @@
       <c r="AK35">
         <v>0</v>
       </c>
-      <c r="AL35">
+      <c r="AL35" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM35" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>2000</v>
       </c>
@@ -5162,23 +5279,23 @@
       <c r="X36" s="6">
         <v>70</v>
       </c>
-      <c r="Y36" s="7">
-        <v>0.24348510638297871</v>
+      <c r="Y36" s="6">
+        <v>0</v>
       </c>
       <c r="Z36" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA36" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB36" s="6">
         <v>353.84</v>
       </c>
-      <c r="AC36" s="8">
+      <c r="AB36" s="8">
         <v>1.6E-2</v>
       </c>
+      <c r="AC36">
+        <v>1</v>
+      </c>
       <c r="AD36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE36">
         <v>0</v>
@@ -5201,11 +5318,14 @@
       <c r="AK36">
         <v>0</v>
       </c>
-      <c r="AL36">
+      <c r="AL36" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>2001</v>
       </c>
@@ -5278,23 +5398,23 @@
       <c r="X37" s="6">
         <v>70</v>
       </c>
-      <c r="Y37" s="7">
-        <v>0.24281984334203657</v>
+      <c r="Y37" s="6">
+        <v>0</v>
       </c>
       <c r="Z37" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA37" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB37" s="6">
         <v>364.46</v>
       </c>
-      <c r="AC37" s="8">
+      <c r="AB37" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="AC37">
+        <v>1</v>
+      </c>
       <c r="AD37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE37">
         <v>0</v>
@@ -5317,11 +5437,14 @@
       <c r="AK37">
         <v>0</v>
       </c>
-      <c r="AL37">
+      <c r="AL37" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM37" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>2002</v>
       </c>
@@ -5394,23 +5517,23 @@
       <c r="X38" s="6">
         <v>70</v>
       </c>
-      <c r="Y38" s="7">
-        <v>0.24207161125319693</v>
+      <c r="Y38" s="6">
+        <v>0</v>
       </c>
       <c r="Z38" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA38" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB38" s="6">
         <v>370.29</v>
       </c>
-      <c r="AC38" s="8">
+      <c r="AB38" s="8">
         <v>0.03</v>
       </c>
+      <c r="AC38">
+        <v>1</v>
+      </c>
       <c r="AD38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE38">
         <v>0</v>
@@ -5433,11 +5556,14 @@
       <c r="AK38">
         <v>0</v>
       </c>
-      <c r="AL38">
+      <c r="AL38" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>2003</v>
       </c>
@@ -5510,23 +5636,23 @@
       <c r="X39" s="6">
         <v>70</v>
       </c>
-      <c r="Y39" s="7">
-        <v>0.24097744360902257</v>
+      <c r="Y39" s="6">
+        <v>0</v>
       </c>
       <c r="Z39" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA39" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB39" s="6">
         <v>382.14</v>
       </c>
-      <c r="AC39" s="8">
+      <c r="AB39" s="8">
         <v>1.6E-2</v>
       </c>
+      <c r="AC39">
+        <v>1</v>
+      </c>
       <c r="AD39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE39">
         <v>0</v>
@@ -5549,11 +5675,14 @@
       <c r="AK39">
         <v>0</v>
       </c>
-      <c r="AL39">
+      <c r="AL39" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM39" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>2004</v>
       </c>
@@ -5626,23 +5755,23 @@
       <c r="X40" s="6">
         <v>70</v>
       </c>
-      <c r="Y40" s="7">
-        <v>0.24123555555555554</v>
+      <c r="Y40" s="6">
+        <v>0</v>
       </c>
       <c r="Z40" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA40" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB40" s="6">
         <v>388.64</v>
       </c>
-      <c r="AC40" s="8">
+      <c r="AB40" s="8">
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="AC40">
+        <v>1</v>
+      </c>
       <c r="AD40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE40">
         <v>0</v>
@@ -5665,11 +5794,14 @@
       <c r="AK40">
         <v>0</v>
       </c>
-      <c r="AL40">
+      <c r="AL40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>2005</v>
       </c>
@@ -5742,23 +5874,23 @@
       <c r="X41" s="6">
         <v>70</v>
       </c>
-      <c r="Y41" s="7">
-        <v>0.24197080291970802</v>
+      <c r="Y41" s="6">
+        <v>0</v>
       </c>
       <c r="Z41" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA41" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB41" s="6">
         <v>397.58</v>
       </c>
-      <c r="AC41" s="8">
+      <c r="AB41" s="8">
         <v>1.7000000000000001E-2</v>
       </c>
+      <c r="AC41">
+        <v>1</v>
+      </c>
       <c r="AD41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE41">
         <v>0</v>
@@ -5781,11 +5913,14 @@
       <c r="AK41">
         <v>0</v>
       </c>
-      <c r="AL41">
+      <c r="AL41" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM41" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>2006</v>
       </c>
@@ -5858,23 +5993,23 @@
       <c r="X42" s="6">
         <v>70</v>
       </c>
-      <c r="Y42" s="7">
-        <v>0.24073539192399049</v>
+      <c r="Y42" s="6">
+        <v>0</v>
       </c>
       <c r="Z42" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA42" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB42" s="6">
         <v>405.93</v>
       </c>
-      <c r="AC42" s="8">
+      <c r="AB42" s="8">
         <v>2.3E-2</v>
       </c>
+      <c r="AC42">
+        <v>1</v>
+      </c>
       <c r="AD42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE42">
         <v>0</v>
@@ -5897,11 +6032,14 @@
       <c r="AK42">
         <v>0</v>
       </c>
-      <c r="AL42">
+      <c r="AL42" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM42" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>2007</v>
       </c>
@@ -5974,23 +6112,23 @@
       <c r="X43" s="6">
         <v>70</v>
       </c>
-      <c r="Y43" s="7">
-        <v>0.23718535469107552</v>
+      <c r="Y43" s="6">
+        <v>0</v>
       </c>
       <c r="Z43" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA43" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB43" s="6">
         <v>414.05</v>
       </c>
-      <c r="AC43" s="8">
+      <c r="AB43" s="8">
         <v>2.1000000000000001E-2</v>
       </c>
+      <c r="AC43">
+        <v>1</v>
+      </c>
       <c r="AD43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE43">
         <v>0</v>
@@ -6013,11 +6151,14 @@
       <c r="AK43">
         <v>0</v>
       </c>
-      <c r="AL43">
+      <c r="AL43" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM43" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>2008</v>
       </c>
@@ -6090,23 +6231,23 @@
       <c r="X44" s="6">
         <v>70</v>
       </c>
-      <c r="Y44" s="7">
-        <v>0.23639198218262808</v>
+      <c r="Y44" s="6">
+        <v>0</v>
       </c>
       <c r="Z44" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA44" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB44" s="6">
         <v>424.4</v>
       </c>
-      <c r="AC44" s="8">
+      <c r="AB44" s="8">
         <v>0.02</v>
       </c>
+      <c r="AC44">
+        <v>1</v>
+      </c>
       <c r="AD44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE44">
         <v>0</v>
@@ -6129,11 +6270,14 @@
       <c r="AK44">
         <v>0</v>
       </c>
-      <c r="AL44">
+      <c r="AL44" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM44" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>2009</v>
       </c>
@@ -6206,23 +6350,23 @@
       <c r="X45" s="6">
         <v>70</v>
       </c>
-      <c r="Y45" s="7">
-        <v>0.23552915766738661</v>
+      <c r="Y45" s="6">
+        <v>0</v>
       </c>
       <c r="Z45" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA45" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB45" s="6">
         <v>426.1</v>
       </c>
-      <c r="AC45" s="8">
+      <c r="AB45" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="AC45">
+        <v>1</v>
+      </c>
       <c r="AD45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE45">
         <v>0</v>
@@ -6245,11 +6389,14 @@
       <c r="AK45">
         <v>0</v>
       </c>
-      <c r="AL45">
+      <c r="AL45" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM45" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>2010</v>
       </c>
@@ -6322,23 +6469,23 @@
       <c r="X46" s="6">
         <v>70</v>
       </c>
-      <c r="Y46" s="7">
-        <v>0.23750084745762709</v>
-      </c>
-      <c r="Z46" s="3">
-        <v>0</v>
+      <c r="Y46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="6">
+        <v>0.75</v>
       </c>
       <c r="AA46" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB46" s="6">
         <v>433.34</v>
       </c>
-      <c r="AC46" s="8">
+      <c r="AB46" s="8">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="AC46">
+        <v>1</v>
+      </c>
       <c r="AD46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE46">
         <v>0</v>
@@ -6361,11 +6508,14 @@
       <c r="AK46">
         <v>0</v>
       </c>
-      <c r="AL46">
+      <c r="AL46" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>2011</v>
       </c>
@@ -6438,23 +6588,23 @@
       <c r="X47" s="6">
         <v>70</v>
       </c>
-      <c r="Y47" s="7">
-        <v>0.23850931677018633</v>
-      </c>
-      <c r="Z47" s="3">
-        <v>0</v>
+      <c r="Y47" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="6">
+        <v>0.75</v>
       </c>
       <c r="AA47" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB47" s="6">
         <v>445.47</v>
       </c>
-      <c r="AC47" s="8">
+      <c r="AB47" s="8">
         <v>1.7000000000000001E-2</v>
       </c>
+      <c r="AC47">
+        <v>1</v>
+      </c>
       <c r="AD47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE47">
         <v>0</v>
@@ -6477,11 +6627,14 @@
       <c r="AK47">
         <v>0</v>
       </c>
-      <c r="AL47">
+      <c r="AL47" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>2012</v>
       </c>
@@ -6557,20 +6710,20 @@
       <c r="Y48" s="3">
         <v>0</v>
       </c>
-      <c r="Z48" s="3">
-        <v>0</v>
+      <c r="Z48" s="6">
+        <v>0.75</v>
       </c>
       <c r="AA48" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB48" s="6">
         <v>453.49</v>
       </c>
-      <c r="AC48" s="8">
+      <c r="AB48" s="8">
         <v>2.8000000000000001E-2</v>
       </c>
+      <c r="AC48">
+        <v>1</v>
+      </c>
       <c r="AD48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE48">
         <v>0</v>
@@ -6593,11 +6746,14 @@
       <c r="AK48">
         <v>0</v>
       </c>
-      <c r="AL48">
+      <c r="AL48" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM48" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>2013</v>
       </c>
@@ -6670,23 +6826,23 @@
       <c r="X49" s="6">
         <v>70</v>
       </c>
-      <c r="Y49" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z49" s="4">
+      <c r="Y49" s="4">
         <v>0.12891520244461424</v>
       </c>
+      <c r="Z49" s="6">
+        <v>0.75</v>
+      </c>
       <c r="AA49" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB49" s="6">
         <v>457.57</v>
       </c>
-      <c r="AC49" s="8">
+      <c r="AB49" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
+      <c r="AC49">
+        <v>1</v>
+      </c>
       <c r="AD49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE49">
         <v>0</v>
@@ -6709,11 +6865,14 @@
       <c r="AK49">
         <v>0</v>
       </c>
-      <c r="AL49">
+      <c r="AL49" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM49" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>2014</v>
       </c>
@@ -6786,23 +6945,23 @@
       <c r="X50" s="6">
         <v>70</v>
       </c>
-      <c r="Y50" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z50" s="4">
+      <c r="Y50" s="4">
         <v>0.12842671614100185</v>
       </c>
+      <c r="Z50" s="6">
+        <v>0.75</v>
+      </c>
       <c r="AA50" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB50" s="6">
         <v>465.81</v>
       </c>
-      <c r="AC50" s="8">
+      <c r="AB50" s="8">
         <v>8.9999999999999993E-3</v>
       </c>
+      <c r="AC50">
+        <v>1</v>
+      </c>
       <c r="AD50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE50">
         <v>0</v>
@@ -6825,11 +6984,14 @@
       <c r="AK50">
         <v>0</v>
       </c>
-      <c r="AL50">
+      <c r="AL50" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM50" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>2015</v>
       </c>
@@ -6902,23 +7064,23 @@
       <c r="X51" s="6">
         <v>70</v>
       </c>
-      <c r="Y51" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="4">
+      <c r="Y51" s="4">
         <v>0.1288332426056977</v>
       </c>
+      <c r="Z51" s="6">
+        <v>0.75</v>
+      </c>
       <c r="AA51" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB51" s="6">
         <v>471.4</v>
       </c>
-      <c r="AC51" s="8">
+      <c r="AB51" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
+      <c r="AC51">
+        <v>1</v>
+      </c>
       <c r="AD51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE51">
         <v>0</v>
@@ -6941,11 +7103,14 @@
       <c r="AK51">
         <v>0</v>
       </c>
-      <c r="AL51">
+      <c r="AL51" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM51" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>2016</v>
       </c>
@@ -7018,23 +7183,23 @@
       <c r="X52" s="6">
         <v>70</v>
       </c>
-      <c r="Y52" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="4">
+      <c r="Y52" s="4">
         <v>0.12881735644381559</v>
       </c>
+      <c r="Z52" s="6">
+        <v>0.75</v>
+      </c>
       <c r="AA52" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB52" s="6">
         <v>471.4</v>
       </c>
-      <c r="AC52" s="8">
+      <c r="AB52" s="8">
         <v>1.2E-2</v>
       </c>
+      <c r="AC52">
+        <v>1</v>
+      </c>
       <c r="AD52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE52">
         <v>0</v>
@@ -7057,11 +7222,14 @@
       <c r="AK52">
         <v>0</v>
       </c>
-      <c r="AL52">
+      <c r="AL52" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM52" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>2017</v>
       </c>
@@ -7134,23 +7302,23 @@
       <c r="X53" s="6">
         <v>70</v>
       </c>
-      <c r="Y53" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z53" s="4">
+      <c r="Y53" s="4">
         <v>0.13035802035802038</v>
       </c>
+      <c r="Z53" s="6">
+        <v>0.75</v>
+      </c>
       <c r="AA53" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB53" s="6">
         <v>478</v>
       </c>
-      <c r="AC53" s="8">
+      <c r="AB53" s="8">
         <v>1.4E-2</v>
       </c>
+      <c r="AC53">
+        <v>1</v>
+      </c>
       <c r="AD53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE53">
         <v>0</v>
@@ -7173,11 +7341,14 @@
       <c r="AK53">
         <v>0</v>
       </c>
-      <c r="AL53">
+      <c r="AL53" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>2018</v>
       </c>
@@ -7250,23 +7421,23 @@
       <c r="X54" s="6">
         <v>70</v>
       </c>
-      <c r="Y54" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="4">
+      <c r="Y54" s="4">
         <v>0.13117857969003008</v>
       </c>
+      <c r="Z54" s="6">
+        <v>0.75</v>
+      </c>
       <c r="AA54" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AB54" s="6">
         <v>485.17</v>
       </c>
-      <c r="AC54" s="8">
+      <c r="AB54" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="AC54">
+        <v>1</v>
+      </c>
       <c r="AD54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE54">
         <v>0</v>
@@ -7289,11 +7460,14 @@
       <c r="AK54">
         <v>0</v>
       </c>
-      <c r="AL54">
+      <c r="AL54" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM54" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>2019</v>
       </c>
@@ -7364,44 +7538,50 @@
       <c r="X55" s="3">
         <v>70</v>
       </c>
+      <c r="Z55" s="9">
+        <v>0.75</v>
+      </c>
       <c r="AA55" s="9">
-        <v>0.75</v>
+        <v>496.36</v>
       </c>
       <c r="AB55" s="9">
-        <v>496.36</v>
-      </c>
-      <c r="AC55" s="9">
         <v>2.3E-2</v>
       </c>
-      <c r="AD55">
+      <c r="AC55">
         <v>1</v>
+      </c>
+      <c r="AD55" s="10">
+        <v>1.5E-3</v>
       </c>
       <c r="AE55" s="10">
         <v>1.5E-3</v>
       </c>
-      <c r="AF55" s="10">
-        <v>1.5E-3</v>
+      <c r="AF55">
+        <v>0</v>
       </c>
       <c r="AG55">
         <v>0</v>
       </c>
-      <c r="AH55">
-        <v>0</v>
-      </c>
-      <c r="AI55" s="10">
+      <c r="AH55" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AJ55">
-        <v>0</v>
+      <c r="AI55">
+        <v>0</v>
+      </c>
+      <c r="AJ55" s="12">
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="AK55" s="12">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="AL55" s="12">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AL55" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AM55" s="15">
+        <v>6.6E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>2020</v>
       </c>
@@ -7477,44 +7657,50 @@
       <c r="X56" s="3">
         <v>70</v>
       </c>
+      <c r="Z56" s="9">
+        <v>0.75</v>
+      </c>
       <c r="AA56" s="9">
-        <v>0.75</v>
+        <v>496.36</v>
       </c>
       <c r="AB56" s="9">
-        <v>496.36</v>
-      </c>
-      <c r="AC56" s="9">
         <v>2.3E-2</v>
       </c>
-      <c r="AD56">
+      <c r="AC56">
         <v>1</v>
+      </c>
+      <c r="AD56" s="10">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AE56" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AF56" s="10">
-        <v>3.0000000000000001E-3</v>
+      <c r="AF56">
+        <v>0</v>
       </c>
       <c r="AG56">
         <v>0</v>
       </c>
-      <c r="AH56">
-        <v>0</v>
-      </c>
-      <c r="AI56" s="10">
+      <c r="AH56" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AJ56">
-        <v>0</v>
+      <c r="AI56">
+        <v>0</v>
+      </c>
+      <c r="AJ56" s="12">
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="AK56" s="12">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="AL56" s="12">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AL56" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AM56" s="15">
+        <v>6.6E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>2021</v>
       </c>
@@ -7590,44 +7776,50 @@
       <c r="X57" s="3">
         <v>70</v>
       </c>
+      <c r="Z57" s="9">
+        <v>0.75</v>
+      </c>
       <c r="AA57" s="9">
-        <v>0.75</v>
+        <v>496.36</v>
       </c>
       <c r="AB57" s="9">
-        <v>496.36</v>
-      </c>
-      <c r="AC57" s="9">
         <v>2.3E-2</v>
       </c>
-      <c r="AD57">
+      <c r="AC57">
         <v>1</v>
+      </c>
+      <c r="AD57" s="10">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AE57" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AF57" s="10">
-        <v>5.0000000000000001E-3</v>
+      <c r="AF57">
+        <v>0</v>
       </c>
       <c r="AG57">
         <v>0</v>
       </c>
-      <c r="AH57">
-        <v>0</v>
-      </c>
-      <c r="AI57" s="10">
+      <c r="AH57" s="10">
         <v>0.01</v>
       </c>
-      <c r="AJ57">
-        <v>0</v>
+      <c r="AI57">
+        <v>0</v>
+      </c>
+      <c r="AJ57" s="12">
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="AK57" s="12">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="AL57" s="12">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AL57" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AM57" s="15">
+        <v>6.6E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>2022</v>
       </c>
@@ -7703,44 +7895,50 @@
       <c r="X58" s="3">
         <v>70</v>
       </c>
+      <c r="Z58" s="9">
+        <v>0.75</v>
+      </c>
       <c r="AA58" s="9">
-        <v>0.75</v>
+        <v>496.36</v>
       </c>
       <c r="AB58" s="9">
-        <v>496.36</v>
-      </c>
-      <c r="AC58" s="9">
         <v>2.3E-2</v>
       </c>
-      <c r="AD58">
+      <c r="AC58">
         <v>1</v>
+      </c>
+      <c r="AD58" s="10">
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="AE58" s="10">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="AF58" s="10">
-        <v>7.4999999999999997E-3</v>
+      <c r="AF58">
+        <v>0</v>
       </c>
       <c r="AG58">
         <v>0</v>
       </c>
-      <c r="AH58">
-        <v>0</v>
-      </c>
-      <c r="AI58" s="10">
+      <c r="AH58" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AJ58">
-        <v>0</v>
+      <c r="AI58">
+        <v>0</v>
+      </c>
+      <c r="AJ58" s="12">
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="AK58" s="12">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="AL58" s="12">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AL58" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AM58" s="15">
+        <v>6.6E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2023</v>
       </c>
@@ -7816,44 +8014,50 @@
       <c r="X59" s="3">
         <v>70</v>
       </c>
+      <c r="Z59" s="9">
+        <v>0.75</v>
+      </c>
       <c r="AA59" s="9">
-        <v>0.75</v>
+        <v>496.36</v>
       </c>
       <c r="AB59" s="9">
-        <v>496.36</v>
-      </c>
-      <c r="AC59" s="9">
         <v>2.3E-2</v>
       </c>
-      <c r="AD59">
+      <c r="AC59">
         <v>1</v>
+      </c>
+      <c r="AD59" s="10">
+        <v>0.01</v>
       </c>
       <c r="AE59" s="10">
         <v>0.01</v>
       </c>
-      <c r="AF59" s="10">
-        <v>0.01</v>
+      <c r="AF59">
+        <v>0</v>
       </c>
       <c r="AG59">
         <v>0</v>
       </c>
-      <c r="AH59">
-        <v>0</v>
-      </c>
-      <c r="AI59" s="10">
+      <c r="AH59" s="10">
         <v>0.02</v>
       </c>
-      <c r="AJ59">
-        <v>0</v>
+      <c r="AI59">
+        <v>0</v>
+      </c>
+      <c r="AJ59" s="12">
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="AK59" s="12">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="AL59" s="12">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AL59" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AM59" s="15">
+        <v>6.6E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>2024</v>
       </c>
@@ -7929,44 +8133,50 @@
       <c r="X60" s="3">
         <v>70</v>
       </c>
+      <c r="Z60" s="9">
+        <v>0.75</v>
+      </c>
       <c r="AA60" s="9">
-        <v>0.75</v>
+        <v>496.36</v>
       </c>
       <c r="AB60" s="9">
-        <v>496.36</v>
-      </c>
-      <c r="AC60" s="9">
         <v>2.3E-2</v>
       </c>
+      <c r="AC60" s="10">
+        <v>1.07</v>
+      </c>
       <c r="AD60" s="10">
-        <v>1.07</v>
+        <v>0.01</v>
       </c>
       <c r="AE60" s="10">
         <v>0.01</v>
       </c>
       <c r="AF60" s="10">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="AG60" s="10">
         <v>0.04</v>
       </c>
       <c r="AH60" s="10">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="AI60" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AJ60" s="10">
         <v>0.08</v>
       </c>
+      <c r="AJ60" s="12">
+        <v>8.3299999999999999E-2</v>
+      </c>
       <c r="AK60" s="12">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="AL60" s="12">
         <v>0.33329999999999999</v>
       </c>
+      <c r="AL60" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AM60" s="15">
+        <v>6.6E-3</v>
+      </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>2025</v>
       </c>
@@ -8042,41 +8252,47 @@
       <c r="X61" s="3">
         <v>70</v>
       </c>
+      <c r="Z61" s="9">
+        <v>0.75</v>
+      </c>
       <c r="AA61" s="9">
-        <v>0.75</v>
+        <v>496.36</v>
       </c>
       <c r="AB61" s="9">
-        <v>496.36</v>
-      </c>
-      <c r="AC61" s="9">
         <v>2.3E-2</v>
       </c>
+      <c r="AC61" s="10">
+        <v>1.1399999999999999</v>
+      </c>
       <c r="AD61" s="10">
-        <v>1.1399999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="AE61" s="10">
         <v>0.01</v>
       </c>
       <c r="AF61" s="10">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="AG61" s="10">
         <v>0.04</v>
       </c>
       <c r="AH61" s="10">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="AI61" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AJ61" s="10">
         <v>0.08</v>
       </c>
+      <c r="AJ61" s="12">
+        <v>8.3299999999999999E-2</v>
+      </c>
       <c r="AK61" s="12">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="AL61" s="12">
         <v>0.33329999999999999</v>
+      </c>
+      <c r="AL61" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AM61" s="15">
+        <v>6.6E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>